<commit_message>
add gini criterion to the RandomForestClassifier()
</commit_message>
<xml_diff>
--- a/row data.xlsx
+++ b/row data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\netanel\My_python_Anaconda\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\netanel\PycharmProjects\analyse-respiratory-diseases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DB1F3F14-4F66-4454-8152-BCBA9E469CA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F95B55-39D4-4B6F-A046-61AE3E518A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28275" yWindow="2415" windowWidth="17280" windowHeight="8970"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fix_data2" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,7 +398,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -513,30 +513,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -584,13 +560,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - הדגשה1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -945,16 +921,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>